<commit_message>
Journal de dev et de test
</commit_message>
<xml_diff>
--- a/Journal_De_Dev.xlsx
+++ b/Journal_De_Dev.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexp\OneDrive\Documents\informatique\Projet-Kartel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Cours\2020-2021\Info\Git Projet\Projet-Kartel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{04D20C17-E28F-49EC-89A8-FBEDFA20233C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E26D7C6C-5C40-44F7-A4D7-4495D56124D1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3BE7ECAC-B5C8-469F-A55E-D83FF09B9100}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{3BE7ECAC-B5C8-469F-A55E-D83FF09B9100}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,86 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="25">
+  <si>
+    <t>Classe</t>
+  </si>
+  <si>
+    <t>Fonction</t>
+  </si>
+  <si>
+    <t>Développeur</t>
+  </si>
+  <si>
+    <t>Etat</t>
+  </si>
+  <si>
+    <t>Argent</t>
+  </si>
+  <si>
+    <t>Fait</t>
+  </si>
+  <si>
+    <t>Boss</t>
+  </si>
+  <si>
+    <t>Gangster</t>
+  </si>
+  <si>
+    <t>Case</t>
+  </si>
+  <si>
+    <t>Affichage</t>
+  </si>
+  <si>
+    <t>Dé</t>
+  </si>
+  <si>
+    <t>Résultat</t>
+  </si>
+  <si>
+    <t>Plateau</t>
+  </si>
+  <si>
+    <t>Afficher</t>
+  </si>
+  <si>
+    <t>Remplissage</t>
+  </si>
+  <si>
+    <t>A faire</t>
+  </si>
+  <si>
+    <t>Prison</t>
+  </si>
+  <si>
+    <t>Joueur</t>
+  </si>
+  <si>
+    <t>Déplacement</t>
+  </si>
+  <si>
+    <t>Inspecteur</t>
+  </si>
+  <si>
+    <t>Capture</t>
+  </si>
+  <si>
+    <t>Jeu</t>
+  </si>
+  <si>
+    <t>Start</t>
+  </si>
+  <si>
+    <t>End</t>
+  </si>
+  <si>
+    <t>Jeton</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -55,8 +135,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -371,12 +457,248 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50BE441B-EF91-4A2B-B4A6-1C10EED9DF4E}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="2"/>
+      <c r="B6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="2"/>
+      <c r="B8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="2"/>
+      <c r="B10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="2"/>
+      <c r="B11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="2"/>
+      <c r="B13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="2"/>
+      <c r="B15" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="2"/>
+      <c r="B17" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="2"/>
+      <c r="B18" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="2"/>
+      <c r="B20" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="2"/>
+      <c r="B21" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="A19:A21"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A16:A18"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>